<commit_message>
Adds performance testing by making a stopwatch demo
</commit_message>
<xml_diff>
--- a/src/com/company/utilities/ExcelDataTime.xlsx
+++ b/src/com/company/utilities/ExcelDataTime.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Test Case</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Flight Page</t>
   </si>
 </sst>
 </file>
@@ -279,7 +282,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -304,6 +307,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>10.444</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>